<commit_message>
life table to age 120
</commit_message>
<xml_diff>
--- a/Data/Winklevoss(6).xlsx
+++ b/Data/Winklevoss(6).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13332" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13332" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="33" r:id="rId1"/>
@@ -23402,7 +23402,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -24609,13 +24609,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B94"/>
+  <dimension ref="A1:B104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomRight" activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -25361,6 +25361,86 @@
         <v>110</v>
       </c>
       <c r="B94" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>111</v>
+      </c>
+      <c r="B95" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>112</v>
+      </c>
+      <c r="B96" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>113</v>
+      </c>
+      <c r="B97" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>114</v>
+      </c>
+      <c r="B98" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>115</v>
+      </c>
+      <c r="B99" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>116</v>
+      </c>
+      <c r="B100" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>117</v>
+      </c>
+      <c r="B101" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>118</v>
+      </c>
+      <c r="B102" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>119</v>
+      </c>
+      <c r="B103" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>120</v>
+      </c>
+      <c r="B104" s="4">
         <v>1</v>
       </c>
     </row>
@@ -25377,7 +25457,7 @@
   <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>

</xml_diff>